<commit_message>
was able to add json files to the backend and dispaly on frontedn
</commit_message>
<xml_diff>
--- a/PropPredictorAI/src/Scraper/EXCEL_PRIZEPICKS_DATA/nfl_prizepicks_data.xlsx
+++ b/PropPredictorAI/src/Scraper/EXCEL_PRIZEPICKS_DATA/nfl_prizepicks_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -28,304 +28,286 @@
     <t>Stat Type</t>
   </si>
   <si>
+    <t>Brock Purdy</t>
+  </si>
+  <si>
+    <t>Geno Smith</t>
+  </si>
+  <si>
+    <t>Trevor Lawrence</t>
+  </si>
+  <si>
+    <t>Caleb Williams</t>
+  </si>
+  <si>
+    <t>Jayden Daniels</t>
+  </si>
+  <si>
     <t>Lamar Jackson</t>
   </si>
   <si>
-    <t>Travis Kelce</t>
+    <t>Kyler Murray</t>
+  </si>
+  <si>
+    <t>Jordan Love</t>
+  </si>
+  <si>
+    <t>Baker Mayfield</t>
+  </si>
+  <si>
+    <t>Deshaun Watson</t>
+  </si>
+  <si>
+    <t>Justin Herbert</t>
+  </si>
+  <si>
+    <t>Bo Nix</t>
+  </si>
+  <si>
+    <t>Kirk Cousins</t>
+  </si>
+  <si>
+    <t>Jared Goff</t>
+  </si>
+  <si>
+    <t>Joe Burrow</t>
+  </si>
+  <si>
+    <t>Josh Allen</t>
+  </si>
+  <si>
+    <t>Aaron Rodgers</t>
+  </si>
+  <si>
+    <t>Deebo Samuel</t>
+  </si>
+  <si>
+    <t>D.K. Metcalf</t>
+  </si>
+  <si>
+    <t>Brandon Aiyuk</t>
+  </si>
+  <si>
+    <t>Jaxon Smith-Njigba</t>
+  </si>
+  <si>
+    <t>Jauan Jennings</t>
+  </si>
+  <si>
+    <t>Tyler Lockett</t>
+  </si>
+  <si>
+    <t>George Kittle</t>
+  </si>
+  <si>
+    <t>Brian Thomas</t>
+  </si>
+  <si>
+    <t>D.J. Moore</t>
+  </si>
+  <si>
+    <t>Christian Kirk</t>
+  </si>
+  <si>
+    <t>Rome Odunze</t>
+  </si>
+  <si>
+    <t>Keenan Allen</t>
+  </si>
+  <si>
+    <t>Cole Kmet</t>
+  </si>
+  <si>
+    <t>Terry McLaurin</t>
+  </si>
+  <si>
+    <t>Zay Flowers</t>
+  </si>
+  <si>
+    <t>Rashod Bateman</t>
+  </si>
+  <si>
+    <t>Zach Ertz</t>
+  </si>
+  <si>
+    <t>Mark Andrews</t>
+  </si>
+  <si>
+    <t>Marvin Harrison</t>
+  </si>
+  <si>
+    <t>Jayden Reed</t>
+  </si>
+  <si>
+    <t>Mike Evans</t>
+  </si>
+  <si>
+    <t>Chris Godwin</t>
+  </si>
+  <si>
+    <t>Cade Otton</t>
+  </si>
+  <si>
+    <t>Amari Cooper</t>
+  </si>
+  <si>
+    <t>DeAndre Hopkins</t>
+  </si>
+  <si>
+    <t>Ladd McConkey</t>
+  </si>
+  <si>
+    <t>Courtland Sutton</t>
+  </si>
+  <si>
+    <t>Pat Freiermuth</t>
+  </si>
+  <si>
+    <t>Brock Bowers</t>
+  </si>
+  <si>
+    <t>Drake London</t>
+  </si>
+  <si>
+    <t>Darnell Mooney</t>
+  </si>
+  <si>
+    <t>Kyle Pitts</t>
+  </si>
+  <si>
+    <t>Amon-Ra St. Brown</t>
+  </si>
+  <si>
+    <t>Jameson Williams</t>
+  </si>
+  <si>
+    <t>Jake Ferguson</t>
+  </si>
+  <si>
+    <t>Sam LaPorta</t>
+  </si>
+  <si>
+    <t>Ja'Marr Chase</t>
+  </si>
+  <si>
+    <t>Tee Higgins</t>
+  </si>
+  <si>
+    <t>Garrett Wilson</t>
+  </si>
+  <si>
+    <t>Allen Lazard</t>
+  </si>
+  <si>
+    <t>Dalton Kincaid</t>
+  </si>
+  <si>
+    <t>Tyler Conklin</t>
   </si>
   <si>
     <t>Derrick Henry</t>
   </si>
   <si>
-    <t>Isiah Pacheco</t>
+    <t>Justice Hill</t>
+  </si>
+  <si>
+    <t>Jordan Mason</t>
+  </si>
+  <si>
+    <t>Isaiah Likely</t>
+  </si>
+  <si>
+    <t>Zach Charbonnet</t>
+  </si>
+  <si>
+    <t>Kenneth Walker III</t>
+  </si>
+  <si>
+    <t>Bucky Irving</t>
+  </si>
+  <si>
+    <t>James Conner</t>
+  </si>
+  <si>
+    <t>Josh Jacobs</t>
+  </si>
+  <si>
+    <t>Saquon Barkley</t>
+  </si>
+  <si>
+    <t>Tony Pollard</t>
+  </si>
+  <si>
+    <t>J.K. Dobbins</t>
   </si>
   <si>
     <t>Bijan Robinson</t>
   </si>
   <si>
-    <t>Tyreek Hill</t>
-  </si>
-  <si>
-    <t>Jonathan Taylor</t>
-  </si>
-  <si>
-    <t>Joe Mixon</t>
+    <t>CeeDee Lamb</t>
+  </si>
+  <si>
+    <t>David Montgomery</t>
+  </si>
+  <si>
+    <t>Rico Dowdle</t>
+  </si>
+  <si>
+    <t>Jahmyr Gibbs</t>
+  </si>
+  <si>
+    <t>James Cook</t>
   </si>
   <si>
     <t>Breece Hall</t>
   </si>
   <si>
-    <t>Zay Flowers</t>
-  </si>
-  <si>
-    <t>Mark Andrews</t>
-  </si>
-  <si>
-    <t>Rashee Rice</t>
-  </si>
-  <si>
-    <t>Xavier Worthy</t>
-  </si>
-  <si>
-    <t>Rashod Bateman</t>
-  </si>
-  <si>
-    <t>Mecole Hardman</t>
-  </si>
-  <si>
-    <t>A.J. Brown</t>
-  </si>
-  <si>
-    <t>Christian Kirk</t>
-  </si>
-  <si>
-    <t>Jaylen Waddle</t>
-  </si>
-  <si>
-    <t>Dalton Kincaid</t>
-  </si>
-  <si>
-    <t>Trey McBride</t>
-  </si>
-  <si>
-    <t>Stefon Diggs</t>
-  </si>
-  <si>
-    <t>Michael Pittman Jr.</t>
-  </si>
-  <si>
-    <t>Tank Dell</t>
-  </si>
-  <si>
-    <t>Nico Collins</t>
-  </si>
-  <si>
-    <t>Ja'Marr Chase</t>
-  </si>
-  <si>
-    <t>Tee Higgins</t>
-  </si>
-  <si>
-    <t>Drake London</t>
-  </si>
-  <si>
-    <t>George Pickens</t>
-  </si>
-  <si>
-    <t>Justin Jefferson</t>
-  </si>
-  <si>
-    <t>Malik Nabers</t>
-  </si>
-  <si>
-    <t>D.J. Moore</t>
-  </si>
-  <si>
-    <t>Diontae Johnson</t>
-  </si>
-  <si>
-    <t>Chris Olave</t>
-  </si>
-  <si>
-    <t>Courtland Sutton</t>
-  </si>
-  <si>
-    <t>D.K. Metcalf</t>
-  </si>
-  <si>
-    <t>Brock Bowers</t>
-  </si>
-  <si>
-    <t>Davante Adams</t>
-  </si>
-  <si>
-    <t>CeeDee Lamb</t>
-  </si>
-  <si>
-    <t>Amari Cooper</t>
-  </si>
-  <si>
-    <t>Mike Evans</t>
-  </si>
-  <si>
-    <t>Terry McLaurin</t>
-  </si>
-  <si>
-    <t>Chris Godwin</t>
-  </si>
-  <si>
-    <t>Amon-Ra St. Brown</t>
-  </si>
-  <si>
-    <t>Cooper Kupp</t>
-  </si>
-  <si>
-    <t>Sam LaPorta</t>
-  </si>
-  <si>
-    <t>Puka Nacua</t>
-  </si>
-  <si>
-    <t>Garrett Wilson</t>
-  </si>
-  <si>
-    <t>Patrick Mahomes</t>
-  </si>
-  <si>
-    <t>Josh Jacobs</t>
-  </si>
-  <si>
-    <t>Jalen Hurts</t>
-  </si>
-  <si>
-    <t>Travis Etienne</t>
-  </si>
-  <si>
-    <t>Kyler Murray</t>
-  </si>
-  <si>
-    <t>James Cook</t>
-  </si>
-  <si>
-    <t>James Conner</t>
-  </si>
-  <si>
-    <t>Anthony Richardson</t>
-  </si>
-  <si>
-    <t>Rhamondre Stevenson</t>
-  </si>
-  <si>
-    <t>Najee Harris</t>
-  </si>
-  <si>
-    <t>Aaron Jones</t>
-  </si>
-  <si>
-    <t>Devin Singletary</t>
-  </si>
-  <si>
-    <t>Alvin Kamara</t>
-  </si>
-  <si>
-    <t>Kenneth Walker III</t>
-  </si>
-  <si>
-    <t>Rachaad White</t>
-  </si>
-  <si>
-    <t>Kyren Williams</t>
-  </si>
-  <si>
-    <t>Christian McCaffrey</t>
-  </si>
-  <si>
-    <t>Harrison Butker</t>
-  </si>
-  <si>
-    <t>Jordan Love</t>
-  </si>
-  <si>
-    <t>Trevor Lawrence</t>
-  </si>
-  <si>
-    <t>Tua Tagovailoa</t>
-  </si>
-  <si>
-    <t>Josh Allen</t>
-  </si>
-  <si>
-    <t>C.J. Stroud</t>
-  </si>
-  <si>
-    <t>Joe Burrow</t>
-  </si>
-  <si>
-    <t>Kirk Cousins</t>
-  </si>
-  <si>
-    <t>Russell Wilson</t>
-  </si>
-  <si>
-    <t>Will Levis</t>
-  </si>
-  <si>
-    <t>Caleb Williams</t>
-  </si>
-  <si>
-    <t>Bryce Young</t>
-  </si>
-  <si>
-    <t>Derek Carr</t>
-  </si>
-  <si>
-    <t>Geno Smith</t>
-  </si>
-  <si>
-    <t>Justin Herbert</t>
-  </si>
-  <si>
-    <t>Dak Prescott</t>
-  </si>
-  <si>
-    <t>Deshaun Watson</t>
-  </si>
-  <si>
-    <t>Baker Mayfield</t>
-  </si>
-  <si>
-    <t>Jared Goff</t>
-  </si>
-  <si>
-    <t>Matthew Stafford</t>
-  </si>
-  <si>
-    <t>Brock Purdy</t>
-  </si>
-  <si>
-    <t>Aaron Rodgers</t>
-  </si>
-  <si>
-    <t>Justin Tucker</t>
-  </si>
-  <si>
-    <t>Sep-5-2024 07:20 PM</t>
-  </si>
-  <si>
-    <t>Sep-8-2024 12:00 PM</t>
-  </si>
-  <si>
-    <t>Sep-9-2024 07:15 PM</t>
-  </si>
-  <si>
-    <t>Sep-6-2024 07:15 PM</t>
-  </si>
-  <si>
-    <t>Sep-8-2024 03:05 PM</t>
-  </si>
-  <si>
-    <t>Sep-8-2024 03:25 PM</t>
-  </si>
-  <si>
-    <t>Sep-8-2024 07:20 PM</t>
-  </si>
-  <si>
-    <t>Pass+Rush+Rec TDs</t>
+    <t>Jason Myers</t>
+  </si>
+  <si>
+    <t>Austin Seibert</t>
+  </si>
+  <si>
+    <t>Oct-10-2024 07:15 PM</t>
+  </si>
+  <si>
+    <t>Oct-13-2024 08:30 AM</t>
+  </si>
+  <si>
+    <t>Oct-13-2024 12:00 PM</t>
+  </si>
+  <si>
+    <t>Oct-13-2024 03:05 PM</t>
+  </si>
+  <si>
+    <t>Oct-13-2024 03:25 PM</t>
+  </si>
+  <si>
+    <t>Oct-13-2024 07:20 PM</t>
+  </si>
+  <si>
+    <t>Oct-14-2024 07:15 PM</t>
+  </si>
+  <si>
+    <t>Pass Yards</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>Pass TDs</t>
+  </si>
+  <si>
+    <t>Receiving Yards</t>
   </si>
   <si>
     <t>Rush+Rec TDs</t>
   </si>
   <si>
-    <t>Receiving Yards</t>
-  </si>
-  <si>
     <t>Rush Yards</t>
   </si>
   <si>
     <t>Kicking Points</t>
-  </si>
-  <si>
-    <t>Pass Yards</t>
   </si>
   <si>
     <t>FG Made</t>
@@ -686,7 +668,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -711,13 +693,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1.5</v>
+        <v>251.5</v>
       </c>
       <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
         <v>91</v>
-      </c>
-      <c r="D2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -725,13 +707,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>254.5</v>
       </c>
       <c r="C3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D3" t="s">
         <v>91</v>
-      </c>
-      <c r="D3" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -739,13 +721,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>223.5</v>
       </c>
       <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
         <v>91</v>
-      </c>
-      <c r="D4" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -753,13 +735,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>224.5</v>
       </c>
       <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
         <v>91</v>
-      </c>
-      <c r="D5" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -767,13 +749,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>219.5</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -781,13 +763,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>215.5</v>
       </c>
       <c r="C7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -795,13 +777,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>233.5</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -809,13 +791,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>259.5</v>
       </c>
       <c r="C9" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D9" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -823,1343 +805,1777 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>234.5</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D10" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>60.5</v>
+        <v>192.5</v>
       </c>
       <c r="C11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" t="s">
         <v>91</v>
-      </c>
-      <c r="D11" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>52.5</v>
+        <v>181.5</v>
       </c>
       <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" t="s">
         <v>91</v>
-      </c>
-      <c r="D12" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>51.5</v>
+        <v>187.5</v>
       </c>
       <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" t="s">
         <v>91</v>
-      </c>
-      <c r="D13" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>60.5</v>
+        <v>232.5</v>
       </c>
       <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" t="s">
         <v>91</v>
-      </c>
-      <c r="D14" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>47.5</v>
+        <v>250.5</v>
       </c>
       <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
         <v>91</v>
-      </c>
-      <c r="D15" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>10.5</v>
+        <v>259.5</v>
       </c>
       <c r="C16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" t="s">
         <v>91</v>
-      </c>
-      <c r="D16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>30.5</v>
+        <v>224.5</v>
       </c>
       <c r="C17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" t="s">
         <v>91</v>
-      </c>
-      <c r="D17" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>18.5</v>
+        <v>222.5</v>
       </c>
       <c r="C18" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
         <v>91</v>
-      </c>
-      <c r="D18" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B19">
-        <v>19.5</v>
+        <v>274.5</v>
       </c>
       <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" t="s">
         <v>91</v>
-      </c>
-      <c r="D19" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B20">
-        <v>80.5</v>
+        <v>224.5</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B21">
-        <v>93.5</v>
+        <v>299.5</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B22">
-        <v>62.5</v>
+        <v>224.5</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B23">
-        <v>67.5</v>
+        <v>299.5</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B24">
-        <v>57.5</v>
+        <v>274.5</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D24" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B25">
-        <v>56.5</v>
+        <v>0.5</v>
       </c>
       <c r="C25" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" t="s">
         <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B26">
-        <v>67.5</v>
+        <v>0.5</v>
       </c>
       <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
         <v>92</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B27">
-        <v>65.5</v>
+        <v>1.5</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B28">
-        <v>61.5</v>
+        <v>1.5</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B29">
-        <v>70.5</v>
+        <v>79.5</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D29" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B30">
-        <v>84.5</v>
+        <v>53.5</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B31">
-        <v>54.5</v>
+        <v>69.5</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D31" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B32">
-        <v>65.5</v>
+        <v>49.5</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B33">
-        <v>60.5</v>
+        <v>63.5</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B34">
-        <v>91.5</v>
+        <v>39.5</v>
       </c>
       <c r="C34" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B35">
-        <v>57.5</v>
+        <v>89.5</v>
       </c>
       <c r="C35" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B36">
-        <v>65.5</v>
+        <v>39.5</v>
       </c>
       <c r="C36" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B37">
-        <v>54.5</v>
+        <v>45.5</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B38">
-        <v>69.5</v>
+        <v>99.5</v>
       </c>
       <c r="C38" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B39">
-        <v>52.5</v>
+        <v>66.5</v>
       </c>
       <c r="C39" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B40">
-        <v>64.5</v>
+        <v>79.5</v>
       </c>
       <c r="C40" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B41">
-        <v>43.5</v>
+        <v>69.5</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D41" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B42">
-        <v>72.5</v>
+        <v>39.5</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B43">
-        <v>95.5</v>
+        <v>79.5</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B44">
-        <v>63.5</v>
+        <v>49.5</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D44" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B45">
-        <v>70.5</v>
+        <v>38.5</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D45" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B46">
-        <v>61.5</v>
+        <v>24.5</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B47">
-        <v>57.5</v>
+        <v>49.5</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="D47" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B48">
-        <v>87.5</v>
+        <v>43.5</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D48" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B49">
-        <v>71.5</v>
+        <v>69.5</v>
       </c>
       <c r="C49" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="B50">
-        <v>58.5</v>
+        <v>39.5</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D50" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="B51">
-        <v>77.5</v>
+        <v>49.5</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="D51" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B52">
-        <v>70.5</v>
+        <v>56.5</v>
       </c>
       <c r="C52" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D52" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B53">
-        <v>61.5</v>
+        <v>56.5</v>
       </c>
       <c r="C53" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D53" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B54">
-        <v>61.5</v>
+        <v>52.5</v>
       </c>
       <c r="C54" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D54" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B55">
-        <v>46.5</v>
+        <v>35.5</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D55" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="B56">
-        <v>17.5</v>
+        <v>43.5</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D56" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B57">
-        <v>62.5</v>
+        <v>27.5</v>
       </c>
       <c r="C57" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D57" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B58">
-        <v>38.5</v>
+        <v>58.5</v>
       </c>
       <c r="C58" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D58" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="B59">
-        <v>61.5</v>
+        <v>53.5</v>
       </c>
       <c r="C59" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D59" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B60">
-        <v>33.5</v>
+        <v>27.5</v>
       </c>
       <c r="C60" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D60" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B61">
-        <v>69.5</v>
+        <v>26.5</v>
       </c>
       <c r="C61" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B62">
-        <v>60.5</v>
+        <v>27.5</v>
       </c>
       <c r="C62" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D62" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B63">
-        <v>75.5</v>
+        <v>56.5</v>
       </c>
       <c r="C63" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D63" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B64">
-        <v>61.5</v>
+        <v>63.5</v>
       </c>
       <c r="C64" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D64" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B65">
-        <v>42.5</v>
+        <v>63.5</v>
       </c>
       <c r="C65" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D65" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B66">
-        <v>56.5</v>
+        <v>63.5</v>
       </c>
       <c r="C66" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D66" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B67">
-        <v>59.5</v>
+        <v>33.5</v>
       </c>
       <c r="C67" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="B68">
-        <v>68.5</v>
+        <v>55.5</v>
       </c>
       <c r="C68" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D68" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B69">
-        <v>69.5</v>
+        <v>39.5</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D69" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B70">
-        <v>53.5</v>
+        <v>42.5</v>
       </c>
       <c r="C70" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D70" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B71">
-        <v>61.5</v>
+        <v>43.5</v>
       </c>
       <c r="C71" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D71" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B72">
-        <v>63.5</v>
+        <v>31.5</v>
       </c>
       <c r="C72" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D72" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="B73">
-        <v>65.5</v>
+        <v>53.5</v>
       </c>
       <c r="C73" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D73" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="B74">
-        <v>77.5</v>
+        <v>62.5</v>
       </c>
       <c r="C74" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D74" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="B75">
-        <v>87.5</v>
+        <v>51.5</v>
       </c>
       <c r="C75" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D75" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="B76">
-        <v>67.5</v>
+        <v>34.5</v>
       </c>
       <c r="C76" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D76" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B77">
-        <v>7.5</v>
+        <v>77.5</v>
       </c>
       <c r="C77" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D77" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B78">
-        <v>221.5</v>
+        <v>46.5</v>
       </c>
       <c r="C78" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B79">
-        <v>263.5</v>
+        <v>49.5</v>
       </c>
       <c r="C79" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D79" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B80">
-        <v>244.5</v>
+        <v>45.5</v>
       </c>
       <c r="C80" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D80" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B81">
-        <v>258.5</v>
+        <v>78.5</v>
       </c>
       <c r="C81" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D81" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B82">
-        <v>249.5</v>
+        <v>54.5</v>
       </c>
       <c r="C82" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D82" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B83">
-        <v>258.5</v>
+        <v>60.5</v>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D83" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B84">
-        <v>232.5</v>
+        <v>35.5</v>
       </c>
       <c r="C84" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D84" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B85">
-        <v>239.5</v>
+        <v>38.5</v>
       </c>
       <c r="C85" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D85" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="B86">
-        <v>209.5</v>
+        <v>33.5</v>
       </c>
       <c r="C86" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D86" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="B87">
-        <v>266.5</v>
+        <v>0.5</v>
       </c>
       <c r="C87" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D87" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="B88">
-        <v>253.5</v>
+        <v>0.5</v>
       </c>
       <c r="C88" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D88" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" t="s">
-        <v>75</v>
+        <v>23</v>
       </c>
       <c r="B89">
-        <v>246.5</v>
+        <v>0.5</v>
       </c>
       <c r="C89" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D89" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="B90">
-        <v>214.5</v>
+        <v>0.5</v>
       </c>
       <c r="C90" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D90" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B91">
-        <v>215.5</v>
+        <v>0.5</v>
       </c>
       <c r="C91" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D91" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" t="s">
-        <v>78</v>
+        <v>26</v>
       </c>
       <c r="B92">
-        <v>237.5</v>
+        <v>0.5</v>
       </c>
       <c r="C92" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D92" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="B93">
-        <v>199.5</v>
+        <v>0.5</v>
       </c>
       <c r="C93" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>8</v>
       </c>
       <c r="B94">
-        <v>228.5</v>
+        <v>0.5</v>
       </c>
       <c r="C94" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D94" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B95">
-        <v>237.5</v>
+        <v>0.5</v>
       </c>
       <c r="C95" t="s">
+        <v>86</v>
+      </c>
+      <c r="D95" t="s">
         <v>95</v>
-      </c>
-      <c r="D95" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="B96">
-        <v>240.5</v>
+        <v>0.5</v>
       </c>
       <c r="C96" t="s">
+        <v>86</v>
+      </c>
+      <c r="D96" t="s">
         <v>95</v>
-      </c>
-      <c r="D96" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="B97">
-        <v>259.5</v>
+        <v>0.5</v>
       </c>
       <c r="C97" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D97" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B98">
-        <v>222.5</v>
+        <v>0.5</v>
       </c>
       <c r="C98" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D98" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B99">
-        <v>244.5</v>
+        <v>1.5</v>
       </c>
       <c r="C99" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D99" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="B100">
-        <v>265.5</v>
+        <v>0.5</v>
       </c>
       <c r="C100" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D100" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="B101">
-        <v>270.5</v>
+        <v>0.5</v>
       </c>
       <c r="C101" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D101" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="B102">
-        <v>246.5</v>
+        <v>0.5</v>
       </c>
       <c r="C102" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D102" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B103">
-        <v>232.5</v>
+        <v>1.5</v>
       </c>
       <c r="C103" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D103" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B104">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C104" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D104" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" t="s">
+        <v>67</v>
+      </c>
+      <c r="B105">
+        <v>0.5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>84</v>
+      </c>
+      <c r="D105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" t="s">
+        <v>65</v>
+      </c>
+      <c r="B106">
+        <v>0.5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>84</v>
+      </c>
+      <c r="D106" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" t="s">
+        <v>65</v>
+      </c>
+      <c r="B107">
+        <v>79.5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>84</v>
+      </c>
+      <c r="D107" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108">
+        <v>54.5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>84</v>
+      </c>
+      <c r="D108" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" t="s">
+        <v>8</v>
+      </c>
+      <c r="B109">
+        <v>53.5</v>
+      </c>
+      <c r="C109" t="s">
+        <v>86</v>
+      </c>
+      <c r="D109" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110">
+        <v>56.5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>86</v>
+      </c>
+      <c r="D110" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" t="s">
+        <v>63</v>
+      </c>
+      <c r="B111">
+        <v>89.5</v>
+      </c>
+      <c r="C111" t="s">
+        <v>86</v>
+      </c>
+      <c r="D111" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>10</v>
+      </c>
+      <c r="B112">
+        <v>35.5</v>
+      </c>
+      <c r="C112" t="s">
+        <v>86</v>
+      </c>
+      <c r="D112" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113">
+        <v>43.5</v>
+      </c>
+      <c r="C113" t="s">
+        <v>86</v>
+      </c>
+      <c r="D113" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" t="s">
+        <v>11</v>
+      </c>
+      <c r="B114">
+        <v>3.5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>86</v>
+      </c>
+      <c r="D114" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" t="s">
+        <v>70</v>
+      </c>
+      <c r="B115">
+        <v>66.5</v>
+      </c>
+      <c r="C115" t="s">
+        <v>86</v>
+      </c>
+      <c r="D115" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" t="s">
+        <v>71</v>
+      </c>
+      <c r="B116">
+        <v>69.5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>86</v>
+      </c>
+      <c r="D116" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" t="s">
+        <v>72</v>
+      </c>
+      <c r="B117">
+        <v>78.5</v>
+      </c>
+      <c r="C117" t="s">
+        <v>86</v>
+      </c>
+      <c r="D117" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" t="s">
+        <v>73</v>
+      </c>
+      <c r="B118">
+        <v>53.5</v>
+      </c>
+      <c r="C118" t="s">
+        <v>86</v>
+      </c>
+      <c r="D118" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" t="s">
+        <v>74</v>
+      </c>
+      <c r="B119">
+        <v>57.5</v>
+      </c>
+      <c r="C119" t="s">
+        <v>87</v>
+      </c>
+      <c r="D119" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" t="s">
+        <v>75</v>
+      </c>
+      <c r="B120">
+        <v>71.5</v>
+      </c>
+      <c r="C120" t="s">
+        <v>88</v>
+      </c>
+      <c r="D120" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" t="s">
+        <v>76</v>
+      </c>
+      <c r="B121">
+        <v>3.5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>88</v>
+      </c>
+      <c r="D121" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" t="s">
+        <v>77</v>
+      </c>
+      <c r="B122">
+        <v>57.5</v>
+      </c>
+      <c r="C122" t="s">
+        <v>88</v>
+      </c>
+      <c r="D122" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" t="s">
+        <v>78</v>
+      </c>
+      <c r="B123">
+        <v>47.5</v>
+      </c>
+      <c r="C123" t="s">
+        <v>88</v>
+      </c>
+      <c r="D123" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" t="s">
+        <v>79</v>
+      </c>
+      <c r="B124">
+        <v>54.5</v>
+      </c>
+      <c r="C124" t="s">
+        <v>88</v>
+      </c>
+      <c r="D124" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" t="s">
+        <v>19</v>
+      </c>
+      <c r="B125">
+        <v>34.5</v>
+      </c>
+      <c r="C125" t="s">
         <v>90</v>
       </c>
-      <c r="B105">
+      <c r="D125" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" t="s">
+        <v>80</v>
+      </c>
+      <c r="B126">
+        <v>58.5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>90</v>
+      </c>
+      <c r="D126" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" t="s">
+        <v>81</v>
+      </c>
+      <c r="B127">
+        <v>53.5</v>
+      </c>
+      <c r="C127" t="s">
+        <v>90</v>
+      </c>
+      <c r="D127" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" t="s">
+        <v>68</v>
+      </c>
+      <c r="B128">
+        <v>79.5</v>
+      </c>
+      <c r="C128" t="s">
+        <v>84</v>
+      </c>
+      <c r="D128" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" t="s">
+        <v>65</v>
+      </c>
+      <c r="B129">
+        <v>99.5</v>
+      </c>
+      <c r="C129" t="s">
+        <v>84</v>
+      </c>
+      <c r="D129" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" t="s">
+        <v>65</v>
+      </c>
+      <c r="B130">
+        <v>59.5</v>
+      </c>
+      <c r="C130" t="s">
+        <v>84</v>
+      </c>
+      <c r="D130" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" t="s">
+        <v>68</v>
+      </c>
+      <c r="B131">
+        <v>39.5</v>
+      </c>
+      <c r="C131" t="s">
+        <v>84</v>
+      </c>
+      <c r="D131" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>68</v>
+      </c>
+      <c r="B132">
+        <v>69.5</v>
+      </c>
+      <c r="C132" t="s">
+        <v>84</v>
+      </c>
+      <c r="D132" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>65</v>
+      </c>
+      <c r="B133">
+        <v>109.5</v>
+      </c>
+      <c r="C133" t="s">
+        <v>84</v>
+      </c>
+      <c r="D133" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" t="s">
+        <v>82</v>
+      </c>
+      <c r="B134">
+        <v>6.5</v>
+      </c>
+      <c r="C134" t="s">
+        <v>84</v>
+      </c>
+      <c r="D134" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>82</v>
+      </c>
+      <c r="B135">
         <v>1.5</v>
       </c>
-      <c r="C105" t="s">
-        <v>91</v>
-      </c>
-      <c r="D105" t="s">
-        <v>104</v>
+      <c r="C135" t="s">
+        <v>84</v>
+      </c>
+      <c r="D135" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" t="s">
+        <v>83</v>
+      </c>
+      <c r="B136">
+        <v>1.5</v>
+      </c>
+      <c r="C136" t="s">
+        <v>86</v>
+      </c>
+      <c r="D136" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>